<commit_message>
Wire loopback, DMA loopback, Sync loopback (with and without guard module) all working with updated selectable CIC/FIR based DUC/DDC. Reduced logic of cordic with serial architecture. Added logic to save raw ADC samples.
</commit_message>
<xml_diff>
--- a/Testing/TestingResults.xlsx
+++ b/Testing/TestingResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\O\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA09F72-3A85-4679-9178-6F8FF2485A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845FBFEB-9A33-40F4-8614-A2AB4D8ACB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="32">
   <si>
     <t>Avg Pow (dBFS)</t>
   </si>
@@ -108,6 +108,30 @@
   </si>
   <si>
     <t>Ifft Gain (dB)</t>
+  </si>
+  <si>
+    <t>FIR DUC</t>
+  </si>
+  <si>
+    <t>CIC DDC</t>
+  </si>
+  <si>
+    <t>CIC DUC</t>
+  </si>
+  <si>
+    <t>FIR DDC</t>
+  </si>
+  <si>
+    <t>0.08169 BER</t>
+  </si>
+  <si>
+    <t>0.026183 BER</t>
+  </si>
+  <si>
+    <t>0.016582 BER</t>
+  </si>
+  <si>
+    <t>Fc: 275 kHz</t>
   </si>
 </sst>
 </file>
@@ -368,6 +392,407 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>5014</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>7372</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>312510</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>2119</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CECDAFC-1809-1ACE-F77E-71028442332A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18262935" y="4218425"/>
+          <a:ext cx="2142311" cy="1729299"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>582705</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>139583</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E391166-E2EA-3DDC-AAC2-8B12185926F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21279971" y="4213413"/>
+          <a:ext cx="2028264" cy="1685994"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>280146</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>187081</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CDE873F-6425-69EE-6C43-82E2EA3A54ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="24283147" y="4213412"/>
+          <a:ext cx="2185147" cy="1733493"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>406483</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6462963B-5E7B-8C53-A629-74BD650EF442}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18848295" y="7306235"/>
+          <a:ext cx="2826952" cy="1456765"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>480146</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EA44B0F-B9AD-3500-101C-1F2EEA7C0FBD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22736736" y="7306235"/>
+          <a:ext cx="2900616" cy="1467971"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>851648</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>504266</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>72817</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F4F0B52-6CF9-80B8-3DDB-CDAD04F70619}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22725530" y="8863853"/>
+          <a:ext cx="2935942" cy="2347611"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>493062</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>73611</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF6465A9-F80C-88B1-6C45-8914FA157102}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26367442" y="7306235"/>
+          <a:ext cx="2913530" cy="1620023"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>400284</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92174FA2-B21C-A53E-AB01-5CE40BB24FC0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="27062206" y="8852647"/>
+          <a:ext cx="2820753" cy="2196353"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>517072</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>156537</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EAAF816-6936-7849-E7B0-8BFAEC3E37E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="23771679" y="8871858"/>
+          <a:ext cx="2966357" cy="2442536"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -633,33 +1058,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T42"/>
+  <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" topLeftCell="T33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AA64" sqref="AA64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" customWidth="1"/>
-    <col min="15" max="15" width="15" customWidth="1"/>
-    <col min="16" max="17" width="18" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" customWidth="1"/>
+    <col min="11" max="11" width="22.5703125" customWidth="1"/>
+    <col min="12" max="12" width="25.28515625" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" customWidth="1"/>
+    <col min="15" max="15" width="20.7109375" customWidth="1"/>
+    <col min="16" max="16" width="22.7109375" customWidth="1"/>
+    <col min="17" max="17" width="18" customWidth="1"/>
     <col min="18" max="18" width="14.5703125" style="2" customWidth="1"/>
     <col min="19" max="19" width="13.5703125" customWidth="1"/>
     <col min="20" max="20" width="11.140625" style="2" customWidth="1"/>
     <col min="21" max="21" width="11.140625" customWidth="1"/>
+    <col min="22" max="22" width="18.28515625" customWidth="1"/>
+    <col min="28" max="28" width="12.85546875" customWidth="1"/>
+    <col min="34" max="34" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -1103,7 +1532,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>22</v>
       </c>
@@ -1123,16 +1552,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="I19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="R23" s="23"/>
       <c r="T23" s="23"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B24" s="20" t="s">
         <v>21</v>
       </c>
@@ -1179,7 +1608,7 @@
       <c r="S24" s="25"/>
       <c r="T24" s="25"/>
     </row>
-    <row r="25" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19" t="s">
         <v>18</v>
       </c>
@@ -1228,8 +1657,17 @@
       <c r="T25" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V25" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>22</v>
       </c>
@@ -1248,12 +1686,21 @@
       <c r="G26" s="24">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V26" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="R32" s="23"/>
       <c r="T32" s="23"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B33" s="20" t="s">
         <v>21</v>
       </c>
@@ -1300,7 +1747,7 @@
       <c r="S33" s="25"/>
       <c r="T33" s="25"/>
     </row>
-    <row r="34" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="19" t="s">
         <v>18</v>
       </c>
@@ -1350,7 +1797,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>22</v>
       </c>
@@ -1370,11 +1817,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:34" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="R39" s="23"/>
       <c r="T39" s="23"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B40" s="20" t="s">
         <v>21</v>
       </c>
@@ -1420,8 +1867,17 @@
       <c r="R40" s="25"/>
       <c r="S40" s="25"/>
       <c r="T40" s="25"/>
-    </row>
-    <row r="41" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V40" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="19" t="s">
         <v>18</v>
       </c>
@@ -1434,7 +1890,7 @@
         <v>-16</v>
       </c>
       <c r="I41" s="2">
-        <v>7.04</v>
+        <v>6.4374000000000002</v>
       </c>
       <c r="J41" s="2">
         <v>9</v>
@@ -1470,8 +1926,17 @@
       <c r="T41" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="42" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V41" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>22</v>
       </c>
@@ -1489,6 +1954,26 @@
       </c>
       <c r="G42" s="24">
         <v>5</v>
+      </c>
+      <c r="V42" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH42" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="V43" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH43" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1501,5 +1986,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>